<commit_message>
Maybe breaking responsibility matric
</commit_message>
<xml_diff>
--- a/Documentation/Responsibility Matrix.xlsx
+++ b/Documentation/Responsibility Matrix.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nvuke\Documents\3. 4th Year Software Eng\2. Second Term Classes\SE 3350 - Software Construction\Ademidun-Hart-Co\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nvuke\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8508"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -418,6 +418,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -427,9 +430,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -747,7 +747,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
@@ -832,11 +832,11 @@
       <c r="AA2" s="1"/>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
@@ -915,7 +915,7 @@
       <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="10" t="s">
         <v>67</v>
       </c>
       <c r="I5" s="3" t="s">
@@ -1959,17 +1959,17 @@
       <c r="AA33" s="1"/>
     </row>
     <row r="34" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="15"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>

</xml_diff>